<commit_message>
Testing a new solution
</commit_message>
<xml_diff>
--- a/data/File-Replacement.xlsx
+++ b/data/File-Replacement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25e7a3c1ff66b367/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\firstgithubrepo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8E1CA1D-D386-43C9-8EAF-54EB801C523A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C58E182-ED14-40FE-AB80-F95F8AEABB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{BAE65CC2-19A5-48AA-8FF5-88CE6D37B7A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Current Name</t>
   </si>
@@ -33,22 +33,46 @@
     <t>New Name</t>
   </si>
   <si>
-    <t>Cold-Drink-Company/Coke2litre</t>
-  </si>
-  <si>
-    <t>Mineral-Water-Company/Coke2litre</t>
-  </si>
-  <si>
-    <t>Cold-Drink-Company/Pepsi250mlcan</t>
-  </si>
-  <si>
-    <t>Beverages-Only-Company/Pepsi250mlcan</t>
-  </si>
-  <si>
-    <t>Cold-Drink-Company/SpriteBottle700ml</t>
-  </si>
-  <si>
-    <t>Mineral-Water-Company/SpriteBottle700ml</t>
+    <t>gk-aks-Digital/firstgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/secondgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/thirdgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/fourthgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/fifthgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/sixthgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Digital/seventhgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Shared/firstgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Confidential/secondgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Confidential/thirdgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Shared/fourthgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Confidential/fifthgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Shared/sixthgithubrepo</t>
+  </si>
+  <si>
+    <t>gk-aks-Shared/seventhgithubrepo</t>
   </si>
 </sst>
 </file>
@@ -400,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C630A72B-F048-402F-8FE5-DB7923D6DCB7}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,23 +449,55 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>